<commit_message>
halaman superadmin and tandai pengguna alumni
</commit_message>
<xml_diff>
--- a/assets/file/Alumni-2.xlsx
+++ b/assets/file/Alumni-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siluni-ts\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07956885-9534-4913-A419-FDAC23F4B145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13931B4E-1779-44C4-AB41-45359204AD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{91B26D3F-09CD-463D-8530-4F7A088E41A1}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nama</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Posisi</t>
+  </si>
+  <si>
+    <t>Jenis Instansi (Lokal/Nasional/Internasional)</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE21F96-7C77-43DE-A6D5-EEE6CC0378D4}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +462,10 @@
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,9 +491,12 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finishing data tracer for guest
</commit_message>
<xml_diff>
--- a/assets/file/Alumni-2.xlsx
+++ b/assets/file/Alumni-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siluni-ts\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13931B4E-1779-44C4-AB41-45359204AD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697D6FF7-5001-4566-8CD9-38DE5FAA51C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{91B26D3F-09CD-463D-8530-4F7A088E41A1}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="15375" windowHeight="7875" xr2:uid="{91B26D3F-09CD-463D-8530-4F7A088E41A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,10 +59,10 @@
     <t>Tahun Lulus</t>
   </si>
   <si>
-    <t>Posisi</t>
-  </si>
-  <si>
-    <t>Jenis Instansi (Lokal/Nasional/Internasional)</t>
+    <t>Skala Instansi (Lokal/Nasional/Internasional)</t>
+  </si>
+  <si>
+    <t>Profesi</t>
   </si>
 </sst>
 </file>
@@ -450,9 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE21F96-7C77-43DE-A6D5-EEE6CC0378D4}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -491,10 +489,10 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>7</v>

</xml_diff>